<commit_message>
Latest Code and Variable Needed
</commit_message>
<xml_diff>
--- a/08.Miscelleneous/ToDo.xlsx
+++ b/08.Miscelleneous/ToDo.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Add more manual payments</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Aggregate Limit of policy</t>
   </si>
   <si>
-    <t>Need to validate with Indu if correct</t>
-  </si>
-  <si>
     <t>Continue on the pay-to and adj combo analysis but for vendors and complete the viz</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">In Pekin Data, TaxID is already populated for many of the contacts and the contacts with different names and same TaxIds also can be found. </t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t xml:space="preserve">Except the following IDs Authority Limits are set for all the adjusters.
@@ -190,23 +184,35 @@
     <t>Waiting for clarification from Indu</t>
   </si>
   <si>
-    <t>Just imported required tables from Pekin data.</t>
-  </si>
-  <si>
-    <t>Complete/ what to do with NAN</t>
-  </si>
-  <si>
-    <t>if multiple tax id  what to do ? In progress</t>
-  </si>
-  <si>
     <t>Haven'treceived log file</t>
+  </si>
+  <si>
+    <t>Filter on HO cases</t>
+  </si>
+  <si>
+    <t>Experience Level Pullin</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Done but not seems useful as per discussion with Deepak</t>
+  </si>
+  <si>
+    <t>Done. Cross check pending</t>
+  </si>
+  <si>
+    <t>Not useful as not a unique region.</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +231,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -308,6 +322,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +642,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -662,10 +679,10 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="72" x14ac:dyDescent="0.3">
@@ -677,10 +694,10 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="10" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -688,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -703,10 +720,10 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="10" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -714,11 +731,11 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -727,14 +744,14 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="9" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -742,11 +759,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -759,7 +776,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -772,7 +789,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -785,7 +802,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -798,7 +815,7 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="9" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -807,11 +824,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -823,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,183 +867,209 @@
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="2:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>49</v>
+      <c r="E7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
+      <c r="E9" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>50</v>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>51</v>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>11</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" t="s">
-        <v>53</v>
+      <c r="E27" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1057,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1065,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>